<commit_message>
.xls ReqsProyectoFDual_v1 updated, new reqs added
</commit_message>
<xml_diff>
--- a/ReqspProyectoFDual_V1.xlsx
+++ b/ReqspProyectoFDual_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farid\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2D5E76-6CA3-45E5-874B-E521EB761701}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF49245A-E13A-40DD-A3A7-4BF94C51356C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A02C390F-C9E6-4B77-986F-EC5ACE46F6C4}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="105">
   <si>
     <t>-El numero de bits es de 8.</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>-El esclavo configura sus registros de manera análoga al maestro y deberá tener el mismo diccionario de mensajes para que sepa interpretar.</t>
-  </si>
-  <si>
-    <t>-Presionar 1 ves en 1 segundo. invierte el valor del pin de salida.</t>
   </si>
   <si>
     <t>-Presionar 2 veces en 1 segundo. genera un PWM de 1Hz.</t>
@@ -203,9 +200,6 @@
     <t>El led sera de baja intensidad color azul - HW</t>
   </si>
   <si>
-    <t>El estado del led se mantendra hasta que vuelva a exitir mas pulsaciones - SW</t>
-  </si>
-  <si>
     <t>-9600 bd</t>
   </si>
   <si>
@@ -255,9 +249,6 @@
   </si>
   <si>
     <t>Nuevo / Consultar con el cliente</t>
-  </si>
-  <si>
-    <t>Duracion de los pwm despùes del pulso - SW</t>
   </si>
   <si>
     <t>Ejecucion ciclica - SW</t>
@@ -425,40 +416,28 @@
     <t>¿Qué va contener el diccionario de msjs?</t>
   </si>
   <si>
-    <t>¿Qué va untdeer el y msjs?</t>
+    <t>¿Qué mensaje de seguridad?</t>
   </si>
   <si>
-    <t>¿Qué va registrostmaneraer msjs?</t>
+    <t>Presionar 1 vez en 1 segundo. invierte el valor del pin de salida.</t>
   </si>
   <si>
-    <t>¿Qué va inviertetvalorer msjs?</t>
+    <t>Tiempo minimo para considerarse boton pulsado de 50ms</t>
   </si>
   <si>
-    <t>¿Qué va generatPWMer msjs?</t>
+    <t>El led permanece apagado, hasta que el boton se pulse</t>
   </si>
   <si>
-    <t>¿Qué va GeneratPWMer msjs?</t>
+    <t>Si el boton es pulsado mas de 1 segundo no se realizara ninguna operación</t>
   </si>
   <si>
-    <t>¿Qué va bajatcolorer msjs?</t>
+    <t>Duracion de los pwm despùes del activarse - SW</t>
   </si>
   <si>
-    <t>¿Qué va sethastaer msjs?</t>
+    <t>En que pines se van a generar los pwm - HW</t>
   </si>
   <si>
-    <t>¿Qué va setmaser msjs?</t>
-  </si>
-  <si>
-    <t>¿Qué va eltempezaraer msjs?</t>
-  </si>
-  <si>
-    <t>¿Qué va despùestpulsoer msjs?</t>
-  </si>
-  <si>
-    <t>¿Qué va enttarjetaer msjs?</t>
-  </si>
-  <si>
-    <t>¿Qué mensaje de seguridad?</t>
+    <t>En que pines se van a generar los pwm - SW</t>
   </si>
 </sst>
 </file>
@@ -914,7 +893,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1047,6 +1026,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1419,10 +1401,10 @@
   <sheetData>
     <row r="1" spans="3:6" ht="14.4" customHeight="1">
       <c r="C1" s="47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="3:6" ht="14.4" customHeight="1">
@@ -1431,122 +1413,122 @@
     </row>
     <row r="3" spans="3:6">
       <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" ht="14.4" customHeight="1">
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" ht="14.4" customHeight="1">
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="3:6" ht="14.4" customHeight="1">
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" ht="14.4" customHeight="1">
-      <c r="C5" s="1" t="s">
+    <row r="7" spans="3:6">
+      <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="3:6">
-      <c r="C6" s="1" t="s">
+    <row r="8" spans="3:6">
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="3:6">
-      <c r="C7" s="1" t="s">
+    <row r="9" spans="3:6">
+      <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="3:6">
-      <c r="C8" s="1" t="s">
+    <row r="10" spans="3:6">
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="3:6">
-      <c r="C9" s="1" t="s">
+    <row r="11" spans="3:6">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="3:6">
-      <c r="C10" s="1" t="s">
+    <row r="12" spans="3:6">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="3:6">
-      <c r="C11" s="1" t="s">
+    <row r="13" spans="3:6">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="3:6">
-      <c r="C12" s="1" t="s">
+    <row r="14" spans="3:6">
+      <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="3:6">
-      <c r="C13" s="1" t="s">
+    <row r="15" spans="3:6">
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="3:6">
-      <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6">
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6">
-      <c r="C16" s="1" t="s">
+    <row r="17" spans="3:6">
+      <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6">
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1561,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D815AF-EB23-485E-ADBC-540B2AA2F226}">
-  <dimension ref="C1:F30"/>
+  <dimension ref="C1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1576,16 +1558,16 @@
   <sheetData>
     <row r="1" spans="3:6">
       <c r="C1" s="47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="48" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" s="48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="3:6">
@@ -1596,25 +1578,25 @@
     </row>
     <row r="3" spans="3:6">
       <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="46"/>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="46"/>
-    </row>
-    <row r="4" spans="3:6">
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="3:6">
@@ -1622,32 +1604,32 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
+      <c r="D6" t="s">
+        <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="3:6">
-      <c r="C6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6">
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="3:6">
@@ -1655,21 +1637,21 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="3:6">
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:6">
@@ -1677,10 +1659,10 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="3:6">
@@ -1688,10 +1670,10 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="3:6">
@@ -1699,13 +1681,13 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="3:6">
@@ -1713,13 +1695,13 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="3:6">
@@ -1727,181 +1709,231 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6">
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="3:6">
-      <c r="C15" s="1" t="s">
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="C16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
-        <v>17</v>
+      <c r="D19" t="s">
+        <v>16</v>
       </c>
-      <c r="E15" t="s">
-        <v>24</v>
+      <c r="E19" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="16" spans="3:6">
-      <c r="C16" s="1" t="s">
-        <v>7</v>
+    <row r="20" spans="3:5">
+      <c r="C20" s="1" t="s">
+        <v>100</v>
       </c>
-      <c r="D16" t="s">
-        <v>17</v>
+      <c r="D20" t="s">
+        <v>16</v>
       </c>
-      <c r="E16" t="s">
-        <v>24</v>
+      <c r="E20" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5">
-      <c r="C18" s="1" t="s">
+    <row r="21" spans="3:5">
+      <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D18" t="s">
-        <v>17</v>
+      <c r="D21" t="s">
+        <v>16</v>
       </c>
-      <c r="E18" t="s">
-        <v>24</v>
+      <c r="E21" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
-      <c r="C19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5">
-      <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5">
-      <c r="C21" s="1" t="s">
+    <row r="22" spans="3:5">
+      <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5">
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="3:5">
       <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
+      <c r="C24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
+      <c r="C27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
-        <v>17</v>
+      <c r="D27" t="s">
+        <v>16</v>
       </c>
-      <c r="E23" t="s">
-        <v>24</v>
+      <c r="E27" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
-      <c r="C24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5">
-      <c r="C25" s="1" t="s">
+    <row r="28" spans="3:5">
+      <c r="C28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D25" t="s">
-        <v>17</v>
+      <c r="D28" t="s">
+        <v>16</v>
       </c>
-      <c r="E25" t="s">
-        <v>43</v>
+      <c r="E28" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
-      <c r="C26" s="1" t="s">
-        <v>48</v>
+    <row r="29" spans="3:5">
+      <c r="C29" s="1" t="s">
+        <v>101</v>
       </c>
-      <c r="D26" t="s">
-        <v>17</v>
+      <c r="D29" t="s">
+        <v>16</v>
       </c>
-      <c r="E26" t="s">
-        <v>43</v>
+      <c r="E29" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
-      <c r="C27" s="1" t="s">
-        <v>49</v>
+    <row r="30" spans="3:5">
+      <c r="C30" s="1" t="s">
+        <v>99</v>
       </c>
-      <c r="D27" t="s">
-        <v>17</v>
+      <c r="D30" t="s">
+        <v>16</v>
       </c>
-      <c r="E27" t="s">
-        <v>43</v>
+      <c r="E30" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
-      <c r="C28" s="1" t="s">
-        <v>50</v>
+    <row r="31" spans="3:5">
+      <c r="C31" s="1" t="s">
+        <v>103</v>
       </c>
-    </row>
-    <row r="29" spans="3:5">
-      <c r="C29" t="s">
-        <v>93</v>
+      <c r="D31" t="s">
+        <v>16</v>
       </c>
-      <c r="D29" s="49" t="s">
-        <v>95</v>
+      <c r="E31" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
-      <c r="C30" t="s">
-        <v>94</v>
+    <row r="32" spans="3:5">
+      <c r="C32" s="1" t="s">
+        <v>104</v>
       </c>
-      <c r="D30" s="49"/>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D29:D30"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D33:D34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1913,7 +1945,7 @@
   <dimension ref="C1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1925,16 +1957,16 @@
   <sheetData>
     <row r="1" spans="3:6">
       <c r="C1" s="47" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="48" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" s="48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="3:6">
@@ -1945,111 +1977,117 @@
     </row>
     <row r="3" spans="3:6">
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="46"/>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="46"/>
-    </row>
-    <row r="4" spans="3:6">
-      <c r="C4" s="1" t="s">
-        <v>19</v>
+      <c r="D6" t="s">
+        <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="E6" t="s">
+        <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6">
-      <c r="C5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6">
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="3:6">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6">
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="3:6">
       <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
+      <c r="D11" t="s">
+        <v>16</v>
       </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6">
-      <c r="C9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6">
-      <c r="C10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6">
-      <c r="C11" s="1" t="s">
-        <v>50</v>
+      <c r="E11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="3:6">
       <c r="C12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
-      <c r="D12" s="49" t="s">
-        <v>95</v>
+      <c r="D12" s="50" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="3:6">
       <c r="C13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
-      <c r="D13" s="49"/>
+      <c r="D13" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2105,14 +2143,14 @@
       <c r="AB1" s="36"/>
     </row>
     <row r="2" spans="1:256" s="38" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
-      <c r="A2" s="53" t="s">
-        <v>92</v>
+      <c r="A2" s="54" t="s">
+        <v>89</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
       <c r="E2" s="45" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="R2" s="36"/>
       <c r="U2" s="36"/>
@@ -2120,14 +2158,14 @@
       <c r="AB2" s="36"/>
     </row>
     <row r="3" spans="1:256" s="38" customFormat="1" ht="87.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="53" t="s">
-        <v>90</v>
+      <c r="A3" s="54" t="s">
+        <v>87</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="R3" s="36"/>
       <c r="U3" s="36"/>
@@ -2135,14 +2173,14 @@
       <c r="AB3" s="36"/>
     </row>
     <row r="4" spans="1:256" s="38" customFormat="1" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="53" t="s">
-        <v>88</v>
+      <c r="A4" s="54" t="s">
+        <v>85</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
@@ -2155,25 +2193,25 @@
       <c r="N4" s="44"/>
       <c r="O4" s="44"/>
       <c r="P4" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="42"/>
       <c r="R4" s="36"/>
-      <c r="S4" s="50" t="s">
-        <v>85</v>
+      <c r="S4" s="51" t="s">
+        <v>82</v>
       </c>
-      <c r="T4" s="52"/>
+      <c r="T4" s="53"/>
       <c r="U4" s="36"/>
-      <c r="V4" s="55" t="s">
-        <v>84</v>
+      <c r="V4" s="56" t="s">
+        <v>81</v>
       </c>
-      <c r="W4" s="56"/>
-      <c r="X4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="58"/>
       <c r="Y4" s="36"/>
-      <c r="Z4" s="50" t="s">
-        <v>83</v>
+      <c r="Z4" s="51" t="s">
+        <v>80</v>
       </c>
-      <c r="AA4" s="51"/>
+      <c r="AA4" s="52"/>
       <c r="AB4" s="36"/>
     </row>
     <row r="5" spans="1:256" s="38" customFormat="1" ht="114.75" customHeight="1" thickTop="1" thickBot="1">
@@ -2183,34 +2221,34 @@
       <c r="D5" s="37"/>
       <c r="E5" s="41"/>
       <c r="F5" s="40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I5" s="40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L5" s="40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M5" s="40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N5" s="40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O5" s="40" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P5" s="37"/>
       <c r="Q5" s="37"/>
@@ -2229,16 +2267,16 @@
     <row r="6" spans="1:256" s="33" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
       <c r="A6" s="37"/>
       <c r="B6" s="37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
@@ -2251,34 +2289,34 @@
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
       <c r="P6" s="37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Q6" s="37" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R6" s="36"/>
       <c r="S6" s="37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="T6" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="U6" s="36"/>
       <c r="V6" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="W6" s="37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="X6" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Y6" s="36"/>
       <c r="Z6" s="37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AA6" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AB6" s="36"/>
       <c r="AC6" s="35"/>
@@ -2516,73 +2554,73 @@
         <v>0</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="R7" s="11"/>
       <c r="S7" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U7" s="11"/>
       <c r="V7" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="W7" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="X7" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Y7" s="14"/>
       <c r="Z7" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AB7" s="11"/>
       <c r="AC7" s="10"/>

</xml_diff>